<commit_message>
EPBDS-9041 fix expected result for primitives. 0 is returned instead of NULL
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Statistics_avg.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Statistics_avg.xlsx
@@ -287,10 +287,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -358,7 +359,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -684,7 +685,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B3:AF105"/>
+  <dimension ref="B3:AE105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F76" workbookViewId="0">
       <selection activeCell="R110" sqref="R110"/>
@@ -692,37 +693,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
-    <col min="2" max="2" width="66.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="79.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9.140625" style="2" collapsed="1"/>
-    <col min="11" max="11" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="10.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.140625" style="2"/>
-    <col min="16" max="16" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="7.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="6.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.7109375" style="2" customWidth="1"/>
-    <col min="21" max="21" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="6.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="9.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="10.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="9.140625" style="2" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="6.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="13" style="2" customWidth="1"/>
-    <col min="33" max="34" width="13" style="2" customWidth="1" collapsed="1"/>
-    <col min="35" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="66.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="2" width="8.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="79.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="9.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="4.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="6.5703125" collapsed="true"/>
+    <col min="10" max="10" style="2" width="9.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="4.7109375" collapsed="true"/>
+    <col min="12" max="14" bestFit="true" customWidth="true" style="2" width="10.140625" collapsed="true"/>
+    <col min="15" max="15" style="2" width="9.140625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="2" width="4.7109375" collapsed="true"/>
+    <col min="17" max="18" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="2" width="6.5703125" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="2" width="18.7109375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="2" width="4.7109375" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="2" width="9.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="2" width="6.5703125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="2" width="9.140625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="2" width="4.7109375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="2" width="20.42578125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="2" width="10.140625" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="2" width="9.140625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="2" width="4.7109375" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="2" width="10.28515625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="2" width="6.5703125" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" style="2" width="13.0" collapsed="true"/>
+    <col min="33" max="34" customWidth="true" style="2" width="13.0" collapsed="true"/>
+    <col min="35" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:31" x14ac:dyDescent="0.25">
@@ -1083,7 +1084,9 @@
       <c r="V8" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="W8" s="5"/>
+      <c r="W8" s="5" t="n">
+        <v>0.0</v>
+      </c>
       <c r="Y8" s="8" t="s">
         <v>50</v>
       </c>
@@ -1266,7 +1269,9 @@
         <v>53</v>
       </c>
       <c r="V11" s="8"/>
-      <c r="W11" s="8"/>
+      <c r="W11" s="8" t="n">
+        <v>0.0</v>
+      </c>
       <c r="Y11" s="5" t="s">
         <v>53</v>
       </c>
@@ -1673,7 +1678,9 @@
       <c r="V21" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="W21" s="5"/>
+      <c r="W21" s="5" t="n">
+        <v>0.0</v>
+      </c>
       <c r="Y21" s="8" t="s">
         <v>50</v>
       </c>
@@ -1856,7 +1863,9 @@
         <v>53</v>
       </c>
       <c r="V24" s="8"/>
-      <c r="W24" s="8"/>
+      <c r="W24" s="8" t="n">
+        <v>0.0</v>
+      </c>
       <c r="Y24" s="5" t="s">
         <v>53</v>
       </c>
@@ -2263,7 +2272,9 @@
       <c r="V34" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="W34" s="5"/>
+      <c r="W34" s="5" t="n">
+        <v>0.0</v>
+      </c>
       <c r="Y34" s="8" t="s">
         <v>50</v>
       </c>
@@ -2446,7 +2457,9 @@
         <v>53</v>
       </c>
       <c r="V37" s="8"/>
-      <c r="W37" s="8"/>
+      <c r="W37" s="8" t="n">
+        <v>0.0</v>
+      </c>
       <c r="Y37" s="5" t="s">
         <v>53</v>
       </c>
@@ -2877,7 +2890,9 @@
       <c r="V47" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="W47" s="5"/>
+      <c r="W47" s="5" t="n">
+        <v>0.0</v>
+      </c>
       <c r="Y47" s="8" t="s">
         <v>50</v>
       </c>
@@ -3060,7 +3075,9 @@
         <v>53</v>
       </c>
       <c r="V50" s="8"/>
-      <c r="W50" s="8"/>
+      <c r="W50" s="8" t="n">
+        <v>0.0</v>
+      </c>
       <c r="Y50" s="5" t="s">
         <v>53</v>
       </c>
@@ -3467,7 +3484,9 @@
       <c r="V60" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="W60" s="5"/>
+      <c r="W60" s="5" t="n">
+        <v>0.0</v>
+      </c>
       <c r="Y60" s="8" t="s">
         <v>50</v>
       </c>
@@ -3650,7 +3669,9 @@
         <v>53</v>
       </c>
       <c r="V63" s="8"/>
-      <c r="W63" s="8"/>
+      <c r="W63" s="8" t="n">
+        <v>0.0</v>
+      </c>
       <c r="Y63" s="5" t="s">
         <v>53</v>
       </c>
@@ -4050,7 +4071,9 @@
       <c r="V73" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="W73" s="5"/>
+      <c r="W73" s="5" t="n">
+        <v>0.0</v>
+      </c>
       <c r="Y73" s="8" t="s">
         <v>50</v>
       </c>
@@ -4233,7 +4256,9 @@
         <v>53</v>
       </c>
       <c r="V76" s="8"/>
-      <c r="W76" s="8"/>
+      <c r="W76" s="8" t="n">
+        <v>0.0</v>
+      </c>
       <c r="Y76" s="5" t="s">
         <v>53</v>
       </c>

</xml_diff>